<commit_message>
v1.1 Changed the owner status accordingly
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_IDCONSTRAINS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_IDCONSTRAINS_REVIEWS.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B273BF-8ACC-444C-B3DA-185B720B0301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name=" LH_TC_IDCONSTRAINS_REVIEWS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
   <si>
     <t>Author</t>
   </si>
@@ -154,11 +155,26 @@
   <si>
     <t xml:space="preserve">initial version of id constrains test cases review </t>
   </si>
+  <si>
+    <t xml:space="preserve">v1.1 </t>
+  </si>
+  <si>
+    <t>Mahmoud Abdelmageed</t>
+  </si>
+  <si>
+    <t>Changed the owner status</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>NotApplicable</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -251,8 +267,308 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -300,310 +616,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
     <dxf>
       <font>
@@ -633,6 +645,10 @@
           <color indexed="64"/>
         </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -663,12 +679,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" name="Date" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -677,20 +693,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review ID" dataDxfId="10"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="9"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="8"/>
-    <tableColumn id="4" name="Version" dataDxfId="7"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="6"/>
-    <tableColumn id="6" name="Actions" dataDxfId="5"/>
-    <tableColumn id="7" name="Owner" dataDxfId="4"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="3"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -739,7 +755,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -791,7 +807,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -992,22 +1008,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1032,47 +1048,56 @@
         <v>32</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D9" ca="1" si="0">TODAY()</f>
+        <f t="shared" ref="D2:D3" ca="1" si="0">TODAY()</f>
         <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1087,29 +1112,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="33.109375" style="5" customWidth="1"/>
     <col min="4" max="4" width="12" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.42578125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="42.28515625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="5"/>
+    <col min="5" max="5" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.44140625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="42.33203125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1141,9 +1166,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.4">
       <c r="A2" s="8">
-        <f t="shared" ref="A2:A12" ca="1" si="0">TODAY()</f>
+        <f t="shared" ref="A2:A5" ca="1" si="0">TODAY()</f>
         <v>45768</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -1168,13 +1193,13 @@
         <v>12</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.4">
       <c r="A3" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45768</v>
@@ -1201,13 +1226,13 @@
         <v>12</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="J3" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="126" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="126" x14ac:dyDescent="0.4">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45768</v>
@@ -1234,13 +1259,13 @@
         <v>12</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="J4" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.4">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45768</v>
@@ -1267,13 +1292,13 @@
         <v>12</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="J5" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1285,7 +1310,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1297,7 +1322,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1309,7 +1334,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1321,7 +1346,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1333,7 +1358,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1345,7 +1370,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1360,13 +1385,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
v1.2 verify the status after modification
verify the status and closed after modification done on the id constraints test cases
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_IDCONSTRAINS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_IDCONSTRAINS_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mego\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\testing\iti\6_QA\workshop\pulled repo\Group-3-Learning-hub-dev\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B273BF-8ACC-444C-B3DA-185B720B0301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
     <sheet name=" LH_TC_IDCONSTRAINS_REVIEWS" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Author</t>
   </si>
@@ -115,9 +114,6 @@
     </r>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>LH_TC_IDCONSTRAINS_REVIEW_002</t>
   </si>
   <si>
@@ -169,12 +165,18 @@
   </si>
   <si>
     <t>NotApplicable</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t>verify the status after modification done on the test cases</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -679,12 +681,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
+    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" name="Date" dataDxfId="12">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -693,20 +695,20 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="9">
+    <tableColumn id="1" name="Date" dataDxfId="9">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1008,22 +1010,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1037,7 +1039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1045,59 +1047,68 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4">
+        <f t="shared" ref="D2:D4" ca="1" si="0">TODAY()</f>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="4">
-        <f t="shared" ref="D2:D3" ca="1" si="0">TODAY()</f>
-        <v>45768</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="D3" s="4">
         <f t="shared" ca="1" si="0"/>
         <v>45768</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" ca="1" si="0"/>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -1112,29 +1123,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="33.109375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="12" style="5" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.44140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="42.33203125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="20.5546875" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="5"/>
+    <col min="5" max="5" width="10.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="42.28515625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="5" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="28.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
@@ -1166,7 +1177,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" ht="105" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <f t="shared" ref="A2:A5" ca="1" si="0">TODAY()</f>
         <v>45768</v>
@@ -1193,22 +1204,22 @@
         <v>12</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="105" x14ac:dyDescent="0.35">
       <c r="A3" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45768</v>
       </c>
       <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>16</v>
@@ -1217,31 +1228,31 @@
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="126" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="126" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45768</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>26</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>16</v>
@@ -1250,28 +1261,28 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>28</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <f t="shared" ca="1" si="0"/>
         <v>45768</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>18</v>
@@ -1283,22 +1294,22 @@
         <v>2</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>12</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -1310,7 +1321,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -1322,7 +1333,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -1334,7 +1345,7 @@
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -1346,7 +1357,7 @@
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -1358,7 +1369,7 @@
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -1370,7 +1381,7 @@
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -1385,13 +1396,13 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>